<commit_message>
1) Fixed a typo 2) Instructions opens to a new tab 3) Arranging folder structure
</commit_message>
<xml_diff>
--- a/Instructions and Documentation/Experiment 27-03-2017/Results Edited.xlsx
+++ b/Instructions and Documentation/Experiment 27-03-2017/Results Edited.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel Dunstan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\I.T Jobs\UWA Ben White Biosecurity Project\Biosecurity Game\Instructions and Documentation\Experiment 27-03-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22044"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>participant.id_in_session</t>
   </si>
@@ -27,9 +27,6 @@
     <t>participant.code</t>
   </si>
   <si>
-    <t>participant.label</t>
-  </si>
-  <si>
     <t>participant._current_app_name</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>b1cup22o</t>
   </si>
   <si>
-    <t>Gabriella</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>ta70guc1</t>
   </si>
   <si>
-    <t>Carolina</t>
-  </si>
-  <si>
     <t>2017-03-27 05:56:35.742290+00:00</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>2hbec6v6</t>
   </si>
   <si>
-    <t>Russell</t>
-  </si>
-  <si>
     <t>2017-03-27 05:58:18.400714+00:00</t>
   </si>
   <si>
@@ -178,9 +166,6 @@
   </si>
   <si>
     <t>13emx8sy</t>
-  </si>
-  <si>
-    <t>Robert</t>
   </si>
   <si>
     <t>2017-03-27 05:58:46.901314+00:00</t>
@@ -192,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,16 +546,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -652,352 +637,337 @@
       <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>58.64</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>58.64</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
         <v>32</v>
       </c>
       <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>35</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2">
+        <v>18</v>
+      </c>
+      <c r="V2" t="s">
         <v>36</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>37</v>
       </c>
-      <c r="V2">
-        <v>18</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
         <v>38</v>
       </c>
-      <c r="X2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>74.48</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="S3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="T3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3">
+        <v>21</v>
+      </c>
+      <c r="V3" t="s">
         <v>43</v>
       </c>
-      <c r="F3">
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>74.48</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V3">
-        <v>21</v>
-      </c>
-      <c r="W3" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" t="s">
-        <v>39</v>
-      </c>
       <c r="Y3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>40</v>
+      <c r="AA3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>106.97</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4">
+        <v>21</v>
+      </c>
+      <c r="V4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
+      <c r="W4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>106.97</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4" t="s">
-        <v>44</v>
-      </c>
-      <c r="T4" t="s">
-        <v>45</v>
-      </c>
-      <c r="U4" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4">
-        <v>21</v>
-      </c>
-      <c r="W4" t="s">
-        <v>51</v>
-      </c>
-      <c r="X4" t="s">
-        <v>39</v>
-      </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
         <v>1</v>
       </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>40</v>
+      <c r="AA4" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>123.3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>123.3</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" t="s">
-        <v>33</v>
-      </c>
       <c r="P5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q5" t="s">
         <v>33</v>
       </c>
       <c r="R5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="T5" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5">
+        <v>22</v>
+      </c>
+      <c r="V5" t="s">
         <v>50</v>
       </c>
-      <c r="V5">
-        <v>22</v>
-      </c>
       <c r="W5" t="s">
-        <v>55</v>
-      </c>
-      <c r="X5" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
         <v>1</v>
       </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>40</v>
+      <c r="AA5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>